<commit_message>
(ADDed SqLite Db, Added Folder structure for Price Data, Put hold on PriceDataApi)
</commit_message>
<xml_diff>
--- a/FinalList.xlsx
+++ b/FinalList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Coin</t>
   </si>
@@ -278,6 +278,108 @@
   </si>
   <si>
     <t>BINANCE_SPOT_BTC_USDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALICEBUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HNTUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RNDRUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EQZUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FORMUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HYVEUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUPERUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ACHUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MLNUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CGGUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ADAUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HBARUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RAYBUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AXSUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUSHIUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DUSKUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CROUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SANDUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LTCUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KCSUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POLSUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATABUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FARMUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MANAUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GENSUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEPUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VRAUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ONEUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PHAUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHIBUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FTMUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BNBUSDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOCGUSDT</t>
+  </si>
+  <si>
+    <t>SymbolDb</t>
   </si>
 </sst>
 </file>
@@ -635,489 +737,466 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>22</v>
+      <c r="A23" t="s">
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>24</v>
+      <c r="A25" t="s">
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>25</v>
+      <c r="A26" t="s">
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>26</v>
+      <c r="A27" t="s">
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>27</v>
+      <c r="A28" t="s">
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>28</v>
+      <c r="A29" t="s">
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>29</v>
+      <c r="A30" t="s">
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>30</v>
+      <c r="A31" t="s">
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>31</v>
+      <c r="A32" t="s">
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>32</v>
+      <c r="A33" t="s">
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>33</v>
+      <c r="A34" t="s">
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1">
-        <v>34</v>
+      <c r="A35" t="s">
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1">
-        <v>35</v>
+      <c r="A36" t="s">
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1">
-        <v>36</v>
+      <c r="A37" t="s">
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>37</v>
+      <c r="A38" t="s">
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>38</v>
+      <c r="A39" t="s">
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>39</v>
+      <c r="A40" t="s">
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1">
-        <v>40</v>
+      <c r="A41" t="s">
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>41</v>
+      <c r="A42" t="s">
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1">
-        <v>42</v>
+      <c r="A43" t="s">
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="1">
-        <v>43</v>
+      <c r="A44" t="s">
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>